<commit_message>
mudança da descrição do reservatorio
</commit_message>
<xml_diff>
--- a/data/identificacao_patu.xlsx
+++ b/data/identificacao_patu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\PycharmProjects\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1486ED4-F0CB-47AA-9CF2-8224E6571D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA05A8E-B98E-4EC3-8F11-F045A2FFA93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,13 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t xml:space="preserve">O Plano de Gestão Proativa de Seca do Hidrossistema Patu foi o primeiro do Ceará e do Brasil, destacando-se por sua metodologia inovadora desenvolvida no âmbito do Programa Cientista Chefe – Recursos Hídricos. Sua elaboração, concluída em 2022, baseou-se em uma construção coletiva e interdisciplinar, envolvendo universidades, colegiados de participação social (como o Comitê de Bacia do Banabuiú e a Comissão Gestora do Açude Patu) e gestores públicos. Esse plano estabeleceu um modelo metodológico que serviu de base para a criação dos demais planos de seca no estado.
-O Hidrossistema Patu está localizado na Região Hidrográfica do Banabuiú, parte da Bacia do Rio Jaguaribe, no município de Senador Pompeu, no Sertão Central do Ceará, uma área severamente afetada pela seca. Seu principal reservatório, o Açude Patu, foi construído em 1987 pelo DNOCS e tem capacidade máxima de 65.103.000 m³, com uma área de drenagem de 993,50 km². O hidrossistema é utilizado para abastecimento humano, irrigação, dessedentação animal e agropecuária. A seca de 2012 impactou significativamente a disponibilidade hídrica e a dinâmica do sistema, levando a restrições de uso e afetando três municípios: Senador Pompeu, Milhã e Quixeramobim. 
-O Sistema de Suporte à Decisão do Plano de Seca do Hidrossistema Patu objetiva ser instrumento de monitoramento, acompanhamento e divulgação das ações pensadas no âmbito do Plano de Seca do Hidrossistema Patu, permitindo uma interface simples, didática e acessível aos distintos atores sociais envolvidos, sobretudo a Câmara Técnica Permanente de Gestão Proativa de Seca da Região Hidrográfica do Banabuiú e a Gerência Regional da Cogerh da Bacia do Banabuiú. 
-Com essa interface, é possível conhecer e acompanhar os distintos estados de seca definidos no plano, as ações sugeridas para serem implementadas em cada um desses estados e a inclusão de novas ações e informações relevantes sobre o estado de seca no hidrossistema.
-</t>
-  </si>
-  <si>
     <t>long</t>
   </si>
   <si>
@@ -71,6 +64,11 @@
   </si>
   <si>
     <t>usos_patu.png</t>
+  </si>
+  <si>
+    <t>O Plano de Gestão Proativa de Seca do Hidrossistema Patu, concluído em 2022, foi o primeiro do Ceará e do Brasil, desenvolvido no âmbito do Programa Cientista Chefe – Recursos Hídricos. Criado de forma coletiva e interdisciplinar, envolveu universidades, colegiados de participação social (Comitê de Bacia do Banabuiú e Comissão Gestora do Açude Patu) e gestores públicos, servindo de modelo para outros planos no estado.
+Localizado no município de Senador Pompeu, no Sertão Central do Ceará, o hidrossistema integra a Região Hidrográfica do Banabuiú, tendo como principal reservatório o Açude Patu, construído em 1987 pelo DNOCS, com capacidade de 65,1 milhões de m³ e área de drenagem de 993,5 km². É usado para abastecimento humano, irrigação, dessedentação animal e agropecuária. A seca de 2012 reduziu drasticamente sua disponibilidade hídrica, afetando também Milhã e Quixeramobim.
+O Sistema de Suporte à Decisão do plano oferece uma interface simples para monitorar e divulgar os estados de seca, as ações previstas para cada cenário e registrar novas medidas, atendendo especialmente à Câmara Técnica Permanente de Gestão Proativa de Seca da Região e à Gerência Regional da Cogerh do Banabuiú.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +474,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -492,48 +490,48 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="173.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="299.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75">

</xml_diff>